<commit_message>
New folder and text file
Created new folder and, within it, a new text file of the use case when
creating a rumor
</commit_message>
<xml_diff>
--- a/Sprint One/Enumerated Lists.xlsx
+++ b/Sprint One/Enumerated Lists.xlsx
@@ -196,11 +196,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +514,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
@@ -522,256 +522,256 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3" t="s">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>